<commit_message>
list1 & list2 completed
</commit_message>
<xml_diff>
--- a/ris_files/result_set.xlsx
+++ b/ris_files/result_set.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/literature/phd_kul/ris_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB766DD-4C94-3C4A-9E57-F93B8B43F95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="39960" yWindow="2000" windowWidth="32460" windowHeight="35600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="383">
   <si>
     <t>type_of_reference</t>
   </si>
@@ -1046,13 +1052,151 @@
   </si>
   <si>
     <t>urn:nbn:de:kobv:517-opus-49222</t>
+  </si>
+  <si>
+    <t>Efficient Vehicle Certification Management with Business Process Management</t>
+  </si>
+  <si>
+    <t>SSRN</t>
+  </si>
+  <si>
+    <t>Balancing Flexibility and Compliance in Response to Long-Tailed Business Process Changes</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Chapter 4: Next-Generation Business Process Management (BPM)</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>excluded: book chapter</t>
+  </si>
+  <si>
+    <t>excluded: different use case</t>
+  </si>
+  <si>
+    <t>excluded: preprint article that has not been peer reviewed.</t>
+  </si>
+  <si>
+    <t>Business Process Reengineering of emergency management procedures: A case study</t>
+  </si>
+  <si>
+    <t>short communication</t>
+  </si>
+  <si>
+    <t>excluded: article type = "chort communication"</t>
+  </si>
+  <si>
+    <t>A knowledge-intensive adaptive business process management framework</t>
+  </si>
+  <si>
+    <t>Research Article</t>
+  </si>
+  <si>
+    <t>The Business Process Management Map – an Effective Means for Managing the Enterprise Value Chain</t>
+  </si>
+  <si>
+    <t>From policy implementation to business process management: Principles for creating flexibility and agility</t>
+  </si>
+  <si>
+    <t>Improved Compliance by BPM-Driven Workflow Automation</t>
+  </si>
+  <si>
+    <t>Improving Telemedicine Processes Via BPM</t>
+  </si>
+  <si>
+    <t>SD1</t>
+  </si>
+  <si>
+    <t>SD2</t>
+  </si>
+  <si>
+    <t>SD3</t>
+  </si>
+  <si>
+    <t>SD4</t>
+  </si>
+  <si>
+    <t>excluded: different concept</t>
+  </si>
+  <si>
+    <t>dblp1</t>
+  </si>
+  <si>
+    <t>dblp2</t>
+  </si>
+  <si>
+    <t>dblp3</t>
+  </si>
+  <si>
+    <t>dblp4</t>
+  </si>
+  <si>
+    <t>dblp5</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>arXiv</t>
+  </si>
+  <si>
+    <t>Efficient Checking of Timed Order Compliance Rules over Graph-encoded Event Logs</t>
+  </si>
+  <si>
+    <t>Non with "Business Process Management on BPM in the title</t>
+  </si>
+  <si>
+    <r>
+      <t>Predictive </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lucida Grande"/>
+        <family val="2"/>
+      </rPr>
+      <t>Compliance Monitoring in Process-Aware Information Systems: State of the Art, Functionalities, Research Directions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Semi-automated checking for regulatory </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Lucida Grande"/>
+        <family val="2"/>
+      </rPr>
+      <t>compliance in e-Health</t>
+    </r>
+  </si>
+  <si>
+    <t>An Open-Source Integration of Process Mining Features into the Camunda Workflow Engine: Data Extraction and Challenges</t>
+  </si>
+  <si>
+    <t>Zenodo</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>dblp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1075,13 +1219,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1115,12 +1276,19 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1128,13 +1296,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1172,7 +1348,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1206,6 +1382,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1240,9 +1417,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1415,1928 +1593,2370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B43" sqref="B2:B43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8.83203125" style="4"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="117" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>105</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>141</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>175</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>230</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="M2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>66</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>95</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>106</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>142</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>176</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>231</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="M3" t="s">
-        <v>302</v>
-      </c>
       <c r="N3" t="s">
+        <v>302</v>
+      </c>
+      <c r="O3" t="s">
         <v>303</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>96</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>107</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>143</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>177</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>232</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="M4" t="s">
-        <v>302</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="N4" t="s">
+        <v>302</v>
+      </c>
+      <c r="P4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>68</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>95</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>108</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>144</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>177</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>233</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="M5" t="s">
-        <v>302</v>
-      </c>
       <c r="N5" t="s">
+        <v>302</v>
+      </c>
+      <c r="O5" t="s">
         <v>303</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>68</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>95</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>109</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>145</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>177</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>234</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M6" t="s">
-        <v>302</v>
-      </c>
       <c r="N6" t="s">
+        <v>302</v>
+      </c>
+      <c r="O6" t="s">
         <v>303</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>97</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>110</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>146</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>177</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>235</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="M7" t="s">
-        <v>302</v>
-      </c>
       <c r="N7" t="s">
+        <v>302</v>
+      </c>
+      <c r="O7" t="s">
         <v>303</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>98</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>111</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>147</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>177</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>236</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="M8" t="s">
-        <v>302</v>
-      </c>
       <c r="N8" t="s">
+        <v>302</v>
+      </c>
+      <c r="O8" t="s">
         <v>303</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>63</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>70</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>99</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>112</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>148</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>178</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>237</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="M9" t="s">
-        <v>302</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="N9" t="s">
+        <v>302</v>
+      </c>
+      <c r="P9" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>71</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>95</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>87</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>149</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>179</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>238</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="M10" t="s">
-        <v>302</v>
-      </c>
       <c r="N10" t="s">
+        <v>302</v>
+      </c>
+      <c r="O10" t="s">
         <v>303</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>100</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>113</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>122</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>179</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>239</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="M11" t="s">
-        <v>302</v>
-      </c>
       <c r="N11" t="s">
+        <v>302</v>
+      </c>
+      <c r="O11" t="s">
         <v>303</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>72</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>95</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>114</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>150</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>180</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>240</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="M12" t="s">
-        <v>302</v>
-      </c>
       <c r="N12" t="s">
+        <v>302</v>
+      </c>
+      <c r="O12" t="s">
         <v>303</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>101</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>115</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>151</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>180</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>241</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="M13" t="s">
-        <v>302</v>
-      </c>
       <c r="N13" t="s">
+        <v>302</v>
+      </c>
+      <c r="O13" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>64</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>74</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>96</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>116</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>152</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>181</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>242</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="M14" t="s">
-        <v>302</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="N14" t="s">
+        <v>302</v>
+      </c>
+      <c r="P14" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>75</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>95</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>117</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>153</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>232</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="M15" t="s">
-        <v>302</v>
-      </c>
       <c r="N15" t="s">
+        <v>302</v>
+      </c>
+      <c r="O15" t="s">
         <v>303</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>76</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>95</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>118</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>154</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>181</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>243</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="M16" t="s">
-        <v>302</v>
-      </c>
       <c r="N16" t="s">
+        <v>302</v>
+      </c>
+      <c r="O16" t="s">
         <v>303</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>97</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>119</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>66</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>181</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>244</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M17" t="s">
-        <v>302</v>
-      </c>
       <c r="N17" t="s">
+        <v>302</v>
+      </c>
+      <c r="O17" t="s">
         <v>303</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>78</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>102</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>120</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>155</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>182</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>245</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="M18" t="s">
-        <v>302</v>
-      </c>
       <c r="N18" t="s">
+        <v>302</v>
+      </c>
+      <c r="O18" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>79</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>95</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>121</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>156</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>182</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>238</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="M19" t="s">
-        <v>302</v>
-      </c>
       <c r="N19" t="s">
+        <v>302</v>
+      </c>
+      <c r="O19" t="s">
         <v>303</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>80</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>103</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>122</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>157</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>182</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>246</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="M20" t="s">
-        <v>302</v>
-      </c>
       <c r="N20" t="s">
+        <v>302</v>
+      </c>
+      <c r="O20" t="s">
         <v>303</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>120</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>158</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>182</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>247</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M21" t="s">
-        <v>302</v>
-      </c>
       <c r="N21" t="s">
+        <v>302</v>
+      </c>
+      <c r="O21" t="s">
         <v>306</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>39</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>81</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>95</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>75</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>159</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>183</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>235</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="M22" t="s">
-        <v>302</v>
-      </c>
       <c r="N22" t="s">
+        <v>302</v>
+      </c>
+      <c r="O22" t="s">
         <v>303</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>40</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>82</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>95</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>123</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>160</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>183</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>240</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="M23" t="s">
-        <v>302</v>
-      </c>
       <c r="N23" t="s">
+        <v>302</v>
+      </c>
+      <c r="O23" t="s">
         <v>303</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C24" t="s">
         <v>16</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>82</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>95</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>124</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>127</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>183</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>238</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="M24" t="s">
-        <v>302</v>
-      </c>
       <c r="N24" t="s">
+        <v>302</v>
+      </c>
+      <c r="O24" t="s">
         <v>303</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>82</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>95</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>125</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>161</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>183</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>238</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="M25" t="s">
-        <v>302</v>
-      </c>
       <c r="N25" t="s">
+        <v>302</v>
+      </c>
+      <c r="O25" t="s">
         <v>303</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C26" t="s">
         <v>16</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>43</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>82</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>95</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>126</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>162</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>183</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>238</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="M26" t="s">
-        <v>302</v>
-      </c>
       <c r="N26" t="s">
+        <v>302</v>
+      </c>
+      <c r="O26" t="s">
         <v>303</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C27" t="s">
         <v>16</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>44</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>83</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>104</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>99</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>183</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>248</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="M27" t="s">
-        <v>302</v>
-      </c>
       <c r="N27" t="s">
+        <v>302</v>
+      </c>
+      <c r="O27" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C28" t="s">
         <v>16</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>45</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>127</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>163</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>183</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>244</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="M28" t="s">
-        <v>302</v>
-      </c>
       <c r="N28" t="s">
+        <v>302</v>
+      </c>
+      <c r="O28" t="s">
         <v>308</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>184</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>249</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M29" t="s">
-        <v>302</v>
-      </c>
       <c r="N29" t="s">
+        <v>302</v>
+      </c>
+      <c r="O29" t="s">
         <v>309</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C30" t="s">
         <v>16</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>47</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>84</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>95</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>128</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>164</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>184</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>250</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="M30" t="s">
-        <v>302</v>
-      </c>
       <c r="N30" t="s">
+        <v>302</v>
+      </c>
+      <c r="O30" t="s">
         <v>303</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>48</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>84</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>95</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>129</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>165</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>184</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>251</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="M31" t="s">
-        <v>302</v>
-      </c>
       <c r="N31" t="s">
+        <v>302</v>
+      </c>
+      <c r="O31" t="s">
         <v>303</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>49</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>85</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>101</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>130</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>166</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>184</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>241</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="M32" t="s">
-        <v>302</v>
-      </c>
       <c r="N32" t="s">
+        <v>302</v>
+      </c>
+      <c r="O32" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C33" t="s">
         <v>16</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>50</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>86</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>95</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>131</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>167</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>184</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>252</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="M33" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M33" t="s">
-        <v>302</v>
-      </c>
       <c r="N33" t="s">
+        <v>302</v>
+      </c>
+      <c r="O33" t="s">
         <v>303</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C34" t="s">
         <v>16</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>51</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>87</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>95</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>132</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>168</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>185</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>253</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="M34" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="M34" t="s">
-        <v>302</v>
-      </c>
       <c r="N34" t="s">
+        <v>302</v>
+      </c>
+      <c r="O34" t="s">
         <v>303</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>88</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>101</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>133</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>169</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>185</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>241</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="M35" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="M35" t="s">
-        <v>302</v>
-      </c>
       <c r="N35" t="s">
+        <v>302</v>
+      </c>
+      <c r="O35" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>53</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>88</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>101</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>134</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>170</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>185</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>241</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="M36" t="s">
-        <v>302</v>
-      </c>
       <c r="N36" t="s">
+        <v>302</v>
+      </c>
+      <c r="O36" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>54</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>89</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>97</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>135</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>171</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>185</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>254</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="M37" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="M37" t="s">
-        <v>302</v>
-      </c>
       <c r="N37" t="s">
+        <v>302</v>
+      </c>
+      <c r="O37" t="s">
         <v>303</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C38" t="s">
         <v>16</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>55</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>90</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>95</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>136</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>172</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>186</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>255</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="M38" t="s">
-        <v>302</v>
-      </c>
       <c r="N38" t="s">
+        <v>302</v>
+      </c>
+      <c r="O38" t="s">
         <v>303</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C39" t="s">
         <v>16</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>56</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>90</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>95</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>137</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>90</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>186</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>256</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="M39" t="s">
-        <v>302</v>
-      </c>
       <c r="N39" t="s">
+        <v>302</v>
+      </c>
+      <c r="O39" t="s">
         <v>303</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C40" t="s">
         <v>16</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>138</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>173</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>186</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>257</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="M40" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="M40" t="s">
-        <v>302</v>
-      </c>
       <c r="N40" t="s">
+        <v>302</v>
+      </c>
+      <c r="O40" t="s">
         <v>310</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C41" t="s">
         <v>16</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>58</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>91</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>104</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>139</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>174</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>186</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>258</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="M41" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="M41" t="s">
-        <v>302</v>
-      </c>
       <c r="N41" t="s">
+        <v>302</v>
+      </c>
+      <c r="O41" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C42" t="s">
         <v>16</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>59</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>92</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>97</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>140</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>131</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>187</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>256</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="M42" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="M42" t="s">
-        <v>302</v>
-      </c>
       <c r="N42" t="s">
+        <v>302</v>
+      </c>
+      <c r="O42" t="s">
         <v>303</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>60</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>93</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>102</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>130</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>79</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>187</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>259</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="M43" t="s">
-        <v>302</v>
-      </c>
       <c r="N43" t="s">
+        <v>302</v>
+      </c>
+      <c r="O43" t="s">
         <v>305</v>
       </c>
     </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D44" t="s">
+        <v>344</v>
+      </c>
+      <c r="E44" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D45" t="s">
+        <v>346</v>
+      </c>
+      <c r="E45" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C46" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E46" t="s">
+        <v>351</v>
+      </c>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C47" t="s">
+        <v>355</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E47" t="s">
+        <v>356</v>
+      </c>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C48" t="s">
+        <v>358</v>
+      </c>
+      <c r="D48" t="s">
+        <v>359</v>
+      </c>
+      <c r="E48" t="s">
+        <v>367</v>
+      </c>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C49" t="s">
+        <v>358</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C50" t="s">
+        <v>358</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C51" t="s">
+        <v>358</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C52" t="s">
+        <v>358</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D53" t="s">
+        <v>375</v>
+      </c>
+      <c r="E53" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D54" t="s">
+        <v>377</v>
+      </c>
+      <c r="E54" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D55" t="s">
+        <v>378</v>
+      </c>
+      <c r="E55" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D56" t="s">
+        <v>379</v>
+      </c>
+      <c r="E56" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>46</v>
+      </c>
+      <c r="E61" t="s">
+        <v>347</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="70" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="L2" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
-    <hyperlink ref="L3" r:id="rId4"/>
-    <hyperlink ref="J4" r:id="rId5"/>
-    <hyperlink ref="L4" r:id="rId6"/>
-    <hyperlink ref="J5" r:id="rId7"/>
-    <hyperlink ref="L5" r:id="rId8"/>
-    <hyperlink ref="J6" r:id="rId9"/>
-    <hyperlink ref="L6" r:id="rId10"/>
-    <hyperlink ref="J7" r:id="rId11"/>
-    <hyperlink ref="L7" r:id="rId12"/>
-    <hyperlink ref="J8" r:id="rId13"/>
-    <hyperlink ref="L8" r:id="rId14"/>
-    <hyperlink ref="J9" r:id="rId15"/>
-    <hyperlink ref="L9" r:id="rId16"/>
-    <hyperlink ref="J10" r:id="rId17"/>
-    <hyperlink ref="L10" r:id="rId18"/>
-    <hyperlink ref="J11" r:id="rId19"/>
-    <hyperlink ref="L11" r:id="rId20"/>
-    <hyperlink ref="J12" r:id="rId21"/>
-    <hyperlink ref="L12" r:id="rId22"/>
-    <hyperlink ref="J13" r:id="rId23"/>
-    <hyperlink ref="L13" r:id="rId24"/>
-    <hyperlink ref="J14" r:id="rId25"/>
-    <hyperlink ref="L14" r:id="rId26"/>
-    <hyperlink ref="J15" r:id="rId27"/>
-    <hyperlink ref="L15" r:id="rId28"/>
-    <hyperlink ref="J16" r:id="rId29"/>
-    <hyperlink ref="L16" r:id="rId30"/>
-    <hyperlink ref="J17" r:id="rId31"/>
-    <hyperlink ref="L17" r:id="rId32"/>
-    <hyperlink ref="J18" r:id="rId33"/>
-    <hyperlink ref="L18" r:id="rId34"/>
-    <hyperlink ref="J19" r:id="rId35"/>
-    <hyperlink ref="L19" r:id="rId36"/>
-    <hyperlink ref="J20" r:id="rId37"/>
-    <hyperlink ref="L20" r:id="rId38"/>
-    <hyperlink ref="J21" r:id="rId39"/>
-    <hyperlink ref="L21" r:id="rId40"/>
-    <hyperlink ref="J22" r:id="rId41"/>
-    <hyperlink ref="L22" r:id="rId42"/>
-    <hyperlink ref="J23" r:id="rId43"/>
-    <hyperlink ref="L23" r:id="rId44"/>
-    <hyperlink ref="J24" r:id="rId45"/>
-    <hyperlink ref="L24" r:id="rId46"/>
-    <hyperlink ref="J25" r:id="rId47"/>
-    <hyperlink ref="L25" r:id="rId48"/>
-    <hyperlink ref="J26" r:id="rId49"/>
-    <hyperlink ref="L26" r:id="rId50"/>
-    <hyperlink ref="J27" r:id="rId51"/>
-    <hyperlink ref="L27" r:id="rId52"/>
-    <hyperlink ref="J28" r:id="rId53"/>
-    <hyperlink ref="L28" r:id="rId54"/>
-    <hyperlink ref="J29" r:id="rId55"/>
-    <hyperlink ref="L29" r:id="rId56"/>
-    <hyperlink ref="J30" r:id="rId57"/>
-    <hyperlink ref="L30" r:id="rId58"/>
-    <hyperlink ref="J31" r:id="rId59"/>
-    <hyperlink ref="L31" r:id="rId60"/>
-    <hyperlink ref="J32" r:id="rId61"/>
-    <hyperlink ref="L32" r:id="rId62"/>
-    <hyperlink ref="J33" r:id="rId63"/>
-    <hyperlink ref="L33" r:id="rId64"/>
-    <hyperlink ref="J34" r:id="rId65"/>
-    <hyperlink ref="L34" r:id="rId66"/>
-    <hyperlink ref="J35" r:id="rId67"/>
-    <hyperlink ref="L35" r:id="rId68"/>
-    <hyperlink ref="J36" r:id="rId69"/>
-    <hyperlink ref="L36" r:id="rId70"/>
-    <hyperlink ref="J37" r:id="rId71"/>
-    <hyperlink ref="L37" r:id="rId72"/>
-    <hyperlink ref="J38" r:id="rId73"/>
-    <hyperlink ref="L38" r:id="rId74"/>
-    <hyperlink ref="J39" r:id="rId75"/>
-    <hyperlink ref="L39" r:id="rId76"/>
-    <hyperlink ref="J40" r:id="rId77"/>
-    <hyperlink ref="L40" r:id="rId78"/>
-    <hyperlink ref="J41" r:id="rId79"/>
-    <hyperlink ref="L41" r:id="rId80"/>
-    <hyperlink ref="J42" r:id="rId81"/>
-    <hyperlink ref="L42" r:id="rId82"/>
-    <hyperlink ref="J43" r:id="rId83"/>
-    <hyperlink ref="L43" r:id="rId84"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="K4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="K5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="K7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="K8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="M8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="K9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="K10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="M10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="K11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="K12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="K13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="K14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="K15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="K16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="M16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="K17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="M18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="K19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="M19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="K20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="M20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="K21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="M21" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="K22" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="M22" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="K23" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="M23" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="K24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="M24" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="K25" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="M25" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="K26" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="M26" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="K27" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="M27" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="K28" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="M28" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="K29" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="M29" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="K30" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="M30" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="K31" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="M31" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="K32" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="M32" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="K33" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="M33" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="K34" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="M34" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="K35" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="M35" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="K36" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="M36" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="K37" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="M37" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="K38" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="M38" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="K39" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="M39" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="K40" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="M40" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="K41" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="M41" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="K42" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="M42" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="K43" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="M43" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="D46" r:id="rId85" display="https://www.sciencedirect.com/science/article/pii/B9780128051603000041" xr:uid="{4A41FC38-1A22-D641-B72E-B2866A351C65}"/>
+    <hyperlink ref="D47" r:id="rId86" display="https://www.sciencedirect.com/science/article/pii/S0925753512000057" xr:uid="{6A3C7A44-C8F6-874C-A57B-0AA9817D1476}"/>
+    <hyperlink ref="D49" r:id="rId87" display="https://www.sciencedirect.com/science/article/pii/S030643792030106X" xr:uid="{85A83487-8790-5A43-9E87-0FD337163F01}"/>
+    <hyperlink ref="D50" r:id="rId88" display="https://www.sciencedirect.com/science/article/pii/S0740624X11000700" xr:uid="{29757D56-409D-834E-A086-1C86F74DDA00}"/>
+    <hyperlink ref="D51" r:id="rId89" display="https://www.sciencedirect.com/science/article/pii/S2472630322015850" xr:uid="{9238E7B9-AB18-D446-9FE1-9458A2A5E62E}"/>
+    <hyperlink ref="D52" r:id="rId90" display="https://www.sciencedirect.com/science/article/pii/S2212017313002892" xr:uid="{77D7202D-9CB5-AE4B-84F7-0177DD649BE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>